<commit_message>
feat(Exercices): partie 1 finie
</commit_message>
<xml_diff>
--- a/exos/marché/Place du marché.xlsx
+++ b/exos/marché/Place du marché.xlsx
@@ -1,24 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px05iql\source\repos\323-Programmation_fonctionnelle\exos\marché\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt04ihk\Documents\GitHub\323-Programmation_fonctionnelle\exos\marché\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BC4E9C-2FFA-4788-BA5A-20C4CC6452F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Disposition" sheetId="2" r:id="rId1"/>
     <sheet name="Produits" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -150,7 +162,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -502,23 +514,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="28.8" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="4.21875" style="2" customWidth="1"/>
-    <col min="2" max="6" width="17.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="2"/>
-    <col min="8" max="16384" width="11.5546875" style="3"/>
+    <col min="1" max="1" width="4.28515625" style="2" customWidth="1"/>
+    <col min="2" max="6" width="17.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="2"/>
+    <col min="8" max="16384" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="2" spans="2:8" ht="63.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:8" ht="63.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="4">
         <v>1</v>
       </c>
@@ -538,10 +550,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="84" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:8" ht="84" customHeight="1" x14ac:dyDescent="0.45">
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="2:8" ht="63.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" ht="63.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="4">
         <v>6</v>
       </c>
@@ -561,10 +573,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="85.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" ht="85.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="2:8" ht="63.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" ht="63.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="4">
         <v>11</v>
       </c>
@@ -590,19 +602,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="K71" sqref="K71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="11.5546875" style="1"/>
+    <col min="6" max="6" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -622,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -642,7 +654,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -663,7 +675,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -684,7 +696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -705,7 +717,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5+1</f>
         <v>2</v>
@@ -726,7 +738,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>A6</f>
         <v>2</v>
@@ -748,7 +760,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ref="A8:A10" si="1">A7</f>
         <v>2</v>
@@ -770,7 +782,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -792,7 +804,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -814,7 +826,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10+1</f>
         <v>3</v>
@@ -835,7 +847,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>A11</f>
         <v>3</v>
@@ -857,7 +869,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ref="A13:A15" si="2">A12</f>
         <v>3</v>
@@ -879,7 +891,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -901,7 +913,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -923,7 +935,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>A15+1</f>
         <v>4</v>
@@ -944,7 +956,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>A16</f>
         <v>4</v>
@@ -966,7 +978,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ref="A18:A20" si="3">A17</f>
         <v>4</v>
@@ -988,7 +1000,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -1010,7 +1022,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -1032,7 +1044,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>A20+1</f>
         <v>5</v>
@@ -1053,7 +1065,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>A21</f>
         <v>5</v>
@@ -1075,7 +1087,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ref="A23:A25" si="4">A22</f>
         <v>5</v>
@@ -1097,7 +1109,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -1119,7 +1131,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -1141,7 +1153,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>A25+1</f>
         <v>6</v>
@@ -1162,7 +1174,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>A26</f>
         <v>6</v>
@@ -1184,7 +1196,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" ref="A28:A30" si="5">A27</f>
         <v>6</v>
@@ -1206,7 +1218,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="5"/>
         <v>6</v>
@@ -1228,7 +1240,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="5"/>
         <v>6</v>
@@ -1250,7 +1262,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>A30+1</f>
         <v>7</v>
@@ -1271,7 +1283,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>A31</f>
         <v>7</v>
@@ -1293,7 +1305,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" ref="A33:A35" si="6">A32</f>
         <v>7</v>
@@ -1315,7 +1327,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="6"/>
         <v>7</v>
@@ -1337,7 +1349,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="6"/>
         <v>7</v>
@@ -1359,7 +1371,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>A35+1</f>
         <v>8</v>
@@ -1380,7 +1392,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>A36</f>
         <v>8</v>
@@ -1402,7 +1414,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" ref="A38:A40" si="7">A37</f>
         <v>8</v>
@@ -1424,7 +1436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="7"/>
         <v>8</v>
@@ -1446,7 +1458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="7"/>
         <v>8</v>
@@ -1468,7 +1480,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>A40+1</f>
         <v>9</v>
@@ -1489,7 +1501,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>A41</f>
         <v>9</v>
@@ -1511,13 +1523,13 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" ref="A43:A45" si="8">A42</f>
         <v>9</v>
       </c>
       <c r="B43" t="str">
-        <f t="shared" si="0"/>
+        <f>B42</f>
         <v>Bovay</v>
       </c>
       <c r="C43" t="s">
@@ -1533,7 +1545,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="8"/>
         <v>9</v>
@@ -1555,7 +1567,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="8"/>
         <v>9</v>
@@ -1577,7 +1589,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <f>A45+1</f>
         <v>10</v>
@@ -1598,7 +1610,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <f>A46</f>
         <v>10</v>
@@ -1620,7 +1632,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" ref="A48:A50" si="9">A47</f>
         <v>10</v>
@@ -1642,7 +1654,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="9"/>
         <v>10</v>
@@ -1664,7 +1676,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="9"/>
         <v>10</v>
@@ -1686,7 +1698,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <f>A50+1</f>
         <v>11</v>
@@ -1707,7 +1719,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <f>A51</f>
         <v>11</v>
@@ -1729,7 +1741,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" ref="A53:A55" si="10">A52</f>
         <v>11</v>
@@ -1751,7 +1763,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="10"/>
         <v>11</v>
@@ -1773,7 +1785,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="10"/>
         <v>11</v>
@@ -1795,7 +1807,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <f>A55+1</f>
         <v>12</v>
@@ -1816,7 +1828,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <f>A56</f>
         <v>12</v>
@@ -1838,7 +1850,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" ref="A58:A60" si="11">A57</f>
         <v>12</v>
@@ -1860,7 +1872,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="11"/>
         <v>12</v>
@@ -1882,7 +1894,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="11"/>
         <v>12</v>
@@ -1904,7 +1916,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <f>A60+1</f>
         <v>13</v>
@@ -1925,7 +1937,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <f>A61</f>
         <v>13</v>
@@ -1947,7 +1959,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" ref="A63:A65" si="12">A62</f>
         <v>13</v>
@@ -1969,7 +1981,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="12"/>
         <v>13</v>
@@ -1991,7 +2003,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="12"/>
         <v>13</v>
@@ -2013,7 +2025,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <f>A65+1</f>
         <v>14</v>
@@ -2034,7 +2046,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <f>A66</f>
         <v>14</v>
@@ -2056,7 +2068,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" ref="A68:A70" si="13">A67</f>
         <v>14</v>
@@ -2078,7 +2090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="13"/>
         <v>14</v>
@@ -2100,7 +2112,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="13"/>
         <v>14</v>
@@ -2122,7 +2134,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <f>A70+1</f>
         <v>15</v>
@@ -2143,7 +2155,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <f>A71</f>
         <v>15</v>
@@ -2165,7 +2177,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" ref="A73:A75" si="15">A72</f>
         <v>15</v>
@@ -2187,7 +2199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="15"/>
         <v>15</v>
@@ -2209,7 +2221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="15"/>
         <v>15</v>
@@ -2513,9 +2525,29 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7454AF30-32CB-44FA-9F7E-0E5A7DA0EF51}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7454AF30-32CB-44FA-9F7E-0E5A7DA0EF51}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB5AEA10-7702-4AE6-919C-780D36645493}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB5AEA10-7702-4AE6-919C-780D36645493}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(exos): partie 2 finie sans classe product
</commit_message>
<xml_diff>
--- a/exos/marché/Place du marché.xlsx
+++ b/exos/marché/Place du marché.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt04ihk\Documents\GitHub\323-Programmation_fonctionnelle\exos\marché\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BC4E9C-2FFA-4788-BA5A-20C4CC6452F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3ED85CE-0E30-4EF4-9519-3D05782FB015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -606,7 +606,7 @@
   <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>